<commit_message>
Ädded new scripts to validate progress bar as part of InstantOpen NewMember
</commit_message>
<xml_diff>
--- a/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_NewMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB99F45-4EFC-4657-8BE4-2AD62C96AAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C82D61-DB90-4C66-8F2D-8C64FD201399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="ProdData" sheetId="4" r:id="rId4"/>
     <sheet name="DataTwo" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="548">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1648,6 +1648,33 @@
   </si>
   <si>
     <t>42355451</t>
+  </si>
+  <si>
+    <t>IO_364_VerifyHomeIconHighlighted</t>
+  </si>
+  <si>
+    <t>IO_365_VerifyProductsProgressBarSelectedOnceStartAsNewMember</t>
+  </si>
+  <si>
+    <t>IO_376_VerifyInformationProgressBarSelectedOnceStartAsNewMember</t>
+  </si>
+  <si>
+    <t>C28333_VerifyInformationProgressBarHighlightedOnCreditCardInfoPage</t>
+  </si>
+  <si>
+    <t>C28334_VerifyInformationProgressBarHighlightedForPersonalLoan</t>
+  </si>
+  <si>
+    <t>C28335_VerifyInformationProgressBarHighlightedForVehicleLoan</t>
+  </si>
+  <si>
+    <t>C28339_VerifyInformationProgressTabHighLightedOnJointOwnerPage</t>
+  </si>
+  <si>
+    <t>56875676</t>
+  </si>
+  <si>
+    <t>01/08/1892</t>
   </si>
 </sst>
 </file>
@@ -1785,7 +1812,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1837,7 +1864,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2039,10 +2066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4065,6 +4092,104 @@
         <v>5</v>
       </c>
       <c r="D133" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>539</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>540</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>541</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>542</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>543</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>544</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>545</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D140" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4201,19 +4326,26 @@
     <hyperlink ref="B131" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
     <hyperlink ref="B132" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
     <hyperlink ref="B133" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B134" r:id="rId132" xr:uid="{3FC154CB-CBC9-42FC-8547-6FFA9A2A7AA7}"/>
+    <hyperlink ref="B135" r:id="rId133" xr:uid="{CEDFB980-178F-48C3-A8F0-ACB55C53284F}"/>
+    <hyperlink ref="B136" r:id="rId134" xr:uid="{4758C07C-1D3D-4A49-B96C-71A47CF9CE8B}"/>
+    <hyperlink ref="B137" r:id="rId135" xr:uid="{227D6EC0-3E69-4C63-8490-D680936C2EBA}"/>
+    <hyperlink ref="B138" r:id="rId136" xr:uid="{D6EB93AB-F106-42A8-A3F8-56FE65DF5AE6}"/>
+    <hyperlink ref="B139" r:id="rId137" xr:uid="{AF7E2B62-F415-4524-A30C-C8E451CA243F}"/>
+    <hyperlink ref="B140" r:id="rId138" xr:uid="{78CA4D0A-A9AC-4D8D-B4A9-8DA1B2285D29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId132"/>
+  <pageSetup orientation="portrait" r:id="rId139"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD101"/>
+  <dimension ref="A1:AD102"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L109" sqref="L109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4231,7 +4363,7 @@
     <col min="14" max="14" width="15.28515625" customWidth="1"/>
     <col min="15" max="15" width="17.28515625" customWidth="1"/>
     <col min="17" max="17" width="12.42578125" customWidth="1"/>
-    <col min="19" max="19" width="23.28515625" customWidth="1"/>
+    <col min="19" max="19" width="30.28515625" customWidth="1"/>
     <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -9195,6 +9327,70 @@
         <v>85</v>
       </c>
       <c r="Z101" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>545</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="J102" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K102" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L102" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M102" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N102" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O102" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P102" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q102" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R102" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S102" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T102" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U102" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="V102" s="6"/>
+      <c r="W102" s="6"/>
+      <c r="X102" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y102" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z102" s="7" t="s">
         <v>82</v>
       </c>
     </row>
@@ -10395,7 +10591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added PromoCode steps to existing scripts and modified as well.
</commit_message>
<xml_diff>
--- a/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_NewMember\src\main\java\com\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE8D109-5A0F-49A0-8DA8-335D8F0DFBB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2924" uniqueCount="589">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1805,7 +1799,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1945,7 +1939,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1997,7 +1991,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2191,18 +2185,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView topLeftCell="B131" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152:D153"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4510,157 +4504,157 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="B84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="B85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="B88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="B90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="B92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B87" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="B93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="B94" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="B95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="B96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="B97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="B98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="B99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="B100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="B101" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="B102" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="B103" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="B104" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="B105" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="B106" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="B107" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="B108" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="B109" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="B110" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="B111" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="B112" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="B113" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="B114" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="B115" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="B116" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="B117" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="B118" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="B119" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="B120" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="B121" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="B122" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="B123" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="B124" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="B125" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="B126" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="B127" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="B128" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="B129" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="B130" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="B131" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="B132" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="B133" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="B134" r:id="rId132" xr:uid="{3FC154CB-CBC9-42FC-8547-6FFA9A2A7AA7}"/>
-    <hyperlink ref="B135" r:id="rId133" xr:uid="{CEDFB980-178F-48C3-A8F0-ACB55C53284F}"/>
-    <hyperlink ref="B136" r:id="rId134" xr:uid="{4758C07C-1D3D-4A49-B96C-71A47CF9CE8B}"/>
-    <hyperlink ref="B137" r:id="rId135" xr:uid="{227D6EC0-3E69-4C63-8490-D680936C2EBA}"/>
-    <hyperlink ref="B138" r:id="rId136" xr:uid="{D6EB93AB-F106-42A8-A3F8-56FE65DF5AE6}"/>
-    <hyperlink ref="B139" r:id="rId137" xr:uid="{AF7E2B62-F415-4524-A30C-C8E451CA243F}"/>
-    <hyperlink ref="B140" r:id="rId138" xr:uid="{C45DB53F-5C33-4DB7-B186-E36BC409CB8F}"/>
-    <hyperlink ref="B141" r:id="rId139" xr:uid="{594F0C19-564C-44A4-A9C9-1F7A84AE608D}"/>
-    <hyperlink ref="B142" r:id="rId140" xr:uid="{B13B2783-38D2-458F-B8CB-76C287121DC5}"/>
-    <hyperlink ref="B143" r:id="rId141" xr:uid="{273E3631-30F0-4979-A3C3-B7192EE9EBC9}"/>
-    <hyperlink ref="B144" r:id="rId142" xr:uid="{C42689B1-5FC8-42A8-B322-21D79D3E6EC8}"/>
-    <hyperlink ref="B145" r:id="rId143" xr:uid="{78027349-D80C-4AD3-A808-2F6713D31663}"/>
-    <hyperlink ref="B146" r:id="rId144" xr:uid="{17FDB5AD-AF67-4ADE-9966-9096C2F0507F}"/>
-    <hyperlink ref="B147" r:id="rId145" xr:uid="{47B397E7-B784-44CB-B6A7-EAC61EA957B5}"/>
-    <hyperlink ref="B148" r:id="rId146" xr:uid="{96274AE7-3DD1-4649-905E-6B4ECE13BCBB}"/>
-    <hyperlink ref="B149" r:id="rId147" xr:uid="{1DA09280-D753-4782-8E01-13BB333B5571}"/>
-    <hyperlink ref="B150" r:id="rId148" xr:uid="{EFB4455D-54E8-4BE8-AB81-99D5384F9ABF}"/>
-    <hyperlink ref="B151" r:id="rId149" xr:uid="{95F9E398-2A1C-469B-8002-828BB72553D7}"/>
-    <hyperlink ref="B152" r:id="rId150" xr:uid="{D6201B87-BBEE-44B3-B7EE-1B3E3B7C2310}"/>
-    <hyperlink ref="B153" r:id="rId151" xr:uid="{FDBEBFC5-5335-494F-917C-A162EBD2A1FF}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B18" r:id="rId16"/>
+    <hyperlink ref="B19" r:id="rId17"/>
+    <hyperlink ref="B20" r:id="rId18"/>
+    <hyperlink ref="B21" r:id="rId19"/>
+    <hyperlink ref="B22" r:id="rId20"/>
+    <hyperlink ref="B23" r:id="rId21"/>
+    <hyperlink ref="B24" r:id="rId22"/>
+    <hyperlink ref="B25" r:id="rId23"/>
+    <hyperlink ref="B26" r:id="rId24"/>
+    <hyperlink ref="B27" r:id="rId25"/>
+    <hyperlink ref="B28" r:id="rId26"/>
+    <hyperlink ref="B29" r:id="rId27"/>
+    <hyperlink ref="B30" r:id="rId28"/>
+    <hyperlink ref="B31" r:id="rId29"/>
+    <hyperlink ref="B32" r:id="rId30"/>
+    <hyperlink ref="B33" r:id="rId31"/>
+    <hyperlink ref="B34" r:id="rId32"/>
+    <hyperlink ref="B35" r:id="rId33"/>
+    <hyperlink ref="B36" r:id="rId34"/>
+    <hyperlink ref="B37" r:id="rId35"/>
+    <hyperlink ref="B38" r:id="rId36"/>
+    <hyperlink ref="B39" r:id="rId37"/>
+    <hyperlink ref="B40" r:id="rId38"/>
+    <hyperlink ref="B41" r:id="rId39"/>
+    <hyperlink ref="B42" r:id="rId40"/>
+    <hyperlink ref="B43" r:id="rId41"/>
+    <hyperlink ref="B44" r:id="rId42"/>
+    <hyperlink ref="B45" r:id="rId43"/>
+    <hyperlink ref="B46" r:id="rId44"/>
+    <hyperlink ref="B47" r:id="rId45"/>
+    <hyperlink ref="B48" r:id="rId46"/>
+    <hyperlink ref="B49" r:id="rId47"/>
+    <hyperlink ref="B50" r:id="rId48"/>
+    <hyperlink ref="B51" r:id="rId49"/>
+    <hyperlink ref="B52" r:id="rId50"/>
+    <hyperlink ref="B53" r:id="rId51"/>
+    <hyperlink ref="B54" r:id="rId52"/>
+    <hyperlink ref="B55" r:id="rId53"/>
+    <hyperlink ref="B56" r:id="rId54"/>
+    <hyperlink ref="B57" r:id="rId55"/>
+    <hyperlink ref="B58" r:id="rId56"/>
+    <hyperlink ref="B59" r:id="rId57"/>
+    <hyperlink ref="B60" r:id="rId58"/>
+    <hyperlink ref="B61" r:id="rId59"/>
+    <hyperlink ref="B62" r:id="rId60"/>
+    <hyperlink ref="B63" r:id="rId61"/>
+    <hyperlink ref="B64" r:id="rId62"/>
+    <hyperlink ref="B65" r:id="rId63"/>
+    <hyperlink ref="B66" r:id="rId64"/>
+    <hyperlink ref="B67" r:id="rId65"/>
+    <hyperlink ref="B68" r:id="rId66"/>
+    <hyperlink ref="B69" r:id="rId67"/>
+    <hyperlink ref="B70" r:id="rId68"/>
+    <hyperlink ref="B71" r:id="rId69"/>
+    <hyperlink ref="B72" r:id="rId70"/>
+    <hyperlink ref="B73" r:id="rId71"/>
+    <hyperlink ref="B74" r:id="rId72"/>
+    <hyperlink ref="B75" r:id="rId73"/>
+    <hyperlink ref="B76" r:id="rId74"/>
+    <hyperlink ref="B77" r:id="rId75"/>
+    <hyperlink ref="B78" r:id="rId76"/>
+    <hyperlink ref="B79" r:id="rId77"/>
+    <hyperlink ref="B80" r:id="rId78"/>
+    <hyperlink ref="B81" r:id="rId79"/>
+    <hyperlink ref="B82" r:id="rId80"/>
+    <hyperlink ref="B83" r:id="rId81"/>
+    <hyperlink ref="B84" r:id="rId82"/>
+    <hyperlink ref="B85" r:id="rId83"/>
+    <hyperlink ref="B86" r:id="rId84"/>
+    <hyperlink ref="B88" r:id="rId85"/>
+    <hyperlink ref="B89" r:id="rId86"/>
+    <hyperlink ref="B90" r:id="rId87"/>
+    <hyperlink ref="B91" r:id="rId88"/>
+    <hyperlink ref="B92" r:id="rId89"/>
+    <hyperlink ref="B87" r:id="rId90"/>
+    <hyperlink ref="B93" r:id="rId91"/>
+    <hyperlink ref="B94" r:id="rId92"/>
+    <hyperlink ref="B95" r:id="rId93"/>
+    <hyperlink ref="B96" r:id="rId94"/>
+    <hyperlink ref="B97" r:id="rId95"/>
+    <hyperlink ref="B98" r:id="rId96"/>
+    <hyperlink ref="B99" r:id="rId97"/>
+    <hyperlink ref="B100" r:id="rId98"/>
+    <hyperlink ref="B101" r:id="rId99"/>
+    <hyperlink ref="B102" r:id="rId100"/>
+    <hyperlink ref="B103" r:id="rId101"/>
+    <hyperlink ref="B104" r:id="rId102"/>
+    <hyperlink ref="B105" r:id="rId103"/>
+    <hyperlink ref="B106" r:id="rId104"/>
+    <hyperlink ref="B107" r:id="rId105"/>
+    <hyperlink ref="B108" r:id="rId106"/>
+    <hyperlink ref="B109" r:id="rId107"/>
+    <hyperlink ref="B110" r:id="rId108"/>
+    <hyperlink ref="B111" r:id="rId109"/>
+    <hyperlink ref="B112" r:id="rId110"/>
+    <hyperlink ref="B113" r:id="rId111"/>
+    <hyperlink ref="B114" r:id="rId112"/>
+    <hyperlink ref="B115" r:id="rId113"/>
+    <hyperlink ref="B116" r:id="rId114"/>
+    <hyperlink ref="B117" r:id="rId115"/>
+    <hyperlink ref="B118" r:id="rId116"/>
+    <hyperlink ref="B119" r:id="rId117"/>
+    <hyperlink ref="B120" r:id="rId118"/>
+    <hyperlink ref="B121" r:id="rId119"/>
+    <hyperlink ref="B122" r:id="rId120"/>
+    <hyperlink ref="B123" r:id="rId121"/>
+    <hyperlink ref="B124" r:id="rId122"/>
+    <hyperlink ref="B125" r:id="rId123"/>
+    <hyperlink ref="B126" r:id="rId124"/>
+    <hyperlink ref="B127" r:id="rId125"/>
+    <hyperlink ref="B128" r:id="rId126"/>
+    <hyperlink ref="B129" r:id="rId127"/>
+    <hyperlink ref="B130" r:id="rId128"/>
+    <hyperlink ref="B131" r:id="rId129"/>
+    <hyperlink ref="B132" r:id="rId130"/>
+    <hyperlink ref="B133" r:id="rId131"/>
+    <hyperlink ref="B134" r:id="rId132"/>
+    <hyperlink ref="B135" r:id="rId133"/>
+    <hyperlink ref="B136" r:id="rId134"/>
+    <hyperlink ref="B137" r:id="rId135"/>
+    <hyperlink ref="B138" r:id="rId136"/>
+    <hyperlink ref="B139" r:id="rId137"/>
+    <hyperlink ref="B140" r:id="rId138"/>
+    <hyperlink ref="B141" r:id="rId139"/>
+    <hyperlink ref="B142" r:id="rId140"/>
+    <hyperlink ref="B143" r:id="rId141"/>
+    <hyperlink ref="B144" r:id="rId142"/>
+    <hyperlink ref="B145" r:id="rId143"/>
+    <hyperlink ref="B146" r:id="rId144"/>
+    <hyperlink ref="B147" r:id="rId145"/>
+    <hyperlink ref="B148" r:id="rId146"/>
+    <hyperlink ref="B149" r:id="rId147"/>
+    <hyperlink ref="B150" r:id="rId148"/>
+    <hyperlink ref="B151" r:id="rId149"/>
+    <hyperlink ref="B152" r:id="rId150"/>
+    <hyperlink ref="B153" r:id="rId151"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId152"/>
@@ -4668,7 +4662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD357452-D04E-4E34-BBEA-FBA2531933C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4746,8 +4740,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7181748D-AD2C-48BB-B746-0A91746B9CE3}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{49C5BEB0-68B1-4EB7-9832-2B40E497716D}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4755,12 +4749,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE111"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H111" sqref="H111"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4787,7 +4781,8 @@
     <col min="27" max="27" width="14.5703125" customWidth="1"/>
     <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.140625" customWidth="1"/>
+    <col min="30" max="30" width="195.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="3" customFormat="1">
@@ -5204,6 +5199,9 @@
       </c>
       <c r="Z14" s="7" t="s">
         <v>82</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -6647,7 +6645,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:30" s="6" customFormat="1">
+    <row r="49" spans="1:31" s="6" customFormat="1">
       <c r="A49" s="6" t="s">
         <v>339</v>
       </c>
@@ -6664,7 +6662,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:30" ht="13.5" customHeight="1">
+    <row r="50" spans="1:31" ht="13.5" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>342</v>
       </c>
@@ -6681,7 +6679,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="51" spans="1:30">
+    <row r="51" spans="1:31">
       <c r="A51" t="s">
         <v>343</v>
       </c>
@@ -6743,7 +6741,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:30">
+    <row r="52" spans="1:31">
       <c r="A52" t="s">
         <v>344</v>
       </c>
@@ -6805,7 +6803,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:30">
+    <row r="53" spans="1:31">
       <c r="A53" s="6" t="s">
         <v>345</v>
       </c>
@@ -6869,8 +6867,11 @@
       <c r="AD53" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="54" spans="1:30">
+      <c r="AE53" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31">
       <c r="A54" s="6" t="s">
         <v>348</v>
       </c>
@@ -6937,8 +6938,11 @@
       <c r="AD54" s="6" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="55" spans="1:30">
+      <c r="AE54" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31">
       <c r="A55" t="s">
         <v>349</v>
       </c>
@@ -7005,8 +7009,11 @@
       <c r="AD55" s="6" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="56" spans="1:30">
+      <c r="AE55" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31">
       <c r="A56" s="6" t="s">
         <v>350</v>
       </c>
@@ -7074,7 +7081,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="57" spans="1:30">
+    <row r="57" spans="1:31">
       <c r="A57" t="s">
         <v>354</v>
       </c>
@@ -7137,7 +7144,7 @@
       </c>
       <c r="AA57" s="6"/>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:31">
       <c r="A58" t="s">
         <v>355</v>
       </c>
@@ -7199,7 +7206,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:30">
+    <row r="59" spans="1:31">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -7263,8 +7270,11 @@
       <c r="AA59" s="6"/>
       <c r="AB59" s="6"/>
       <c r="AC59" s="6"/>
-    </row>
-    <row r="60" spans="1:30">
+      <c r="AE59" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31">
       <c r="A60" t="s">
         <v>363</v>
       </c>
@@ -7323,7 +7333,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:30">
+    <row r="61" spans="1:31">
       <c r="A61" t="s">
         <v>365</v>
       </c>
@@ -7385,7 +7395,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:30">
+    <row r="62" spans="1:31">
       <c r="A62" s="6" t="s">
         <v>366</v>
       </c>
@@ -7399,7 +7409,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:30">
+    <row r="63" spans="1:31">
       <c r="A63" t="s">
         <v>367</v>
       </c>
@@ -7413,7 +7423,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:30">
+    <row r="64" spans="1:31">
       <c r="A64" s="6" t="s">
         <v>368</v>
       </c>
@@ -8504,7 +8514,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:26">
+    <row r="81" spans="1:31">
       <c r="A81" s="6" t="s">
         <v>508</v>
       </c>
@@ -8568,7 +8578,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="1:26" s="6" customFormat="1">
+    <row r="82" spans="1:31" s="6" customFormat="1">
       <c r="A82" s="6" t="s">
         <v>513</v>
       </c>
@@ -8626,8 +8636,11 @@
       <c r="Z82" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:26" s="6" customFormat="1">
+      <c r="AE82" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="83" spans="1:31" s="6" customFormat="1">
       <c r="A83" s="6" t="s">
         <v>514</v>
       </c>
@@ -8685,8 +8698,11 @@
       <c r="Z83" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:26" s="6" customFormat="1">
+      <c r="AE83" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="84" spans="1:31" s="6" customFormat="1">
       <c r="A84" s="6" t="s">
         <v>515</v>
       </c>
@@ -8745,7 +8761,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:26" s="6" customFormat="1">
+    <row r="85" spans="1:31" s="6" customFormat="1">
       <c r="A85" s="6" t="s">
         <v>516</v>
       </c>
@@ -8803,8 +8819,11 @@
       <c r="Z85" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="86" spans="1:26" s="6" customFormat="1">
+      <c r="AE85" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="86" spans="1:31" s="6" customFormat="1">
       <c r="A86" s="6" t="s">
         <v>517</v>
       </c>
@@ -8862,8 +8881,11 @@
       <c r="Z86" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="87" spans="1:26" s="6" customFormat="1">
+      <c r="AE86" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="87" spans="1:31" s="6" customFormat="1">
       <c r="A87" s="6" t="s">
         <v>518</v>
       </c>
@@ -8922,7 +8944,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:26" s="6" customFormat="1">
+    <row r="88" spans="1:31" s="6" customFormat="1">
       <c r="A88" s="6" t="s">
         <v>519</v>
       </c>
@@ -8981,7 +9003,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:26" s="6" customFormat="1">
+    <row r="89" spans="1:31" s="6" customFormat="1">
       <c r="A89" s="6" t="s">
         <v>520</v>
       </c>
@@ -9040,7 +9062,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:26" s="6" customFormat="1">
+    <row r="90" spans="1:31" s="6" customFormat="1">
       <c r="A90" s="6" t="s">
         <v>523</v>
       </c>
@@ -9099,7 +9121,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="1:26" s="6" customFormat="1">
+    <row r="91" spans="1:31" s="6" customFormat="1">
       <c r="A91" s="6" t="s">
         <v>525</v>
       </c>
@@ -9158,7 +9180,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="92" spans="1:26" s="6" customFormat="1">
+    <row r="92" spans="1:31" s="6" customFormat="1">
       <c r="A92" s="6" t="s">
         <v>526</v>
       </c>
@@ -9217,7 +9239,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="93" spans="1:26" s="6" customFormat="1">
+    <row r="93" spans="1:31" s="6" customFormat="1">
       <c r="A93" s="6" t="s">
         <v>527</v>
       </c>
@@ -9276,7 +9298,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:26" s="6" customFormat="1">
+    <row r="94" spans="1:31" s="6" customFormat="1">
       <c r="A94" s="6" t="s">
         <v>528</v>
       </c>
@@ -9334,8 +9356,11 @@
       <c r="Z94" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="95" spans="1:26" s="6" customFormat="1">
+      <c r="AE94" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="95" spans="1:31" s="6" customFormat="1">
       <c r="A95" s="6" t="s">
         <v>529</v>
       </c>
@@ -9394,7 +9419,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="96" spans="1:26" s="6" customFormat="1">
+    <row r="96" spans="1:31" s="6" customFormat="1">
       <c r="A96" s="6" t="s">
         <v>530</v>
       </c>
@@ -9451,6 +9476,9 @@
       </c>
       <c r="Z96" s="7" t="s">
         <v>82</v>
+      </c>
+      <c r="AE96" s="6" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="97" spans="1:31" s="6" customFormat="1">
@@ -9570,6 +9598,9 @@
       <c r="Z98" s="7" t="s">
         <v>82</v>
       </c>
+      <c r="AE98" s="6" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="99" spans="1:31" s="6" customFormat="1">
       <c r="A99" s="6" t="s">
@@ -9628,6 +9659,9 @@
       </c>
       <c r="Z99" s="7" t="s">
         <v>82</v>
+      </c>
+      <c r="AE99" s="6" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="100" spans="1:31" s="6" customFormat="1">
@@ -10323,16 +10357,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S102" r:id="rId1" xr:uid="{F371BD80-5669-4853-851A-82712007E820}"/>
-    <hyperlink ref="S103" r:id="rId2" xr:uid="{BEE0A138-2C1D-425C-87DE-8ABDC07B8BA6}"/>
-    <hyperlink ref="S104" r:id="rId3" xr:uid="{BB02CF50-90FC-4C40-B952-0DF0F5ED2E0C}"/>
-    <hyperlink ref="S105" r:id="rId4" xr:uid="{878D5BC4-656B-4ED1-AB31-987E46E2594E}"/>
-    <hyperlink ref="S106" r:id="rId5" xr:uid="{59859151-C0CF-4EA6-812B-9964F59A3F94}"/>
-    <hyperlink ref="S107" r:id="rId6" xr:uid="{95873862-68F8-4640-A30C-ECC753AAF49F}"/>
-    <hyperlink ref="S108" r:id="rId7" xr:uid="{68112E65-98BF-4F0F-B34B-26C400A37517}"/>
-    <hyperlink ref="S109" r:id="rId8" xr:uid="{3FED822B-A866-41C0-820B-95A5EF5D2C08}"/>
-    <hyperlink ref="S110" r:id="rId9" xr:uid="{9E6340EB-D4C8-4605-B9BB-161D57EBD0FA}"/>
-    <hyperlink ref="S111" r:id="rId10" xr:uid="{4824B1C4-79BA-436E-93A8-31B164D74736}"/>
+    <hyperlink ref="S102" r:id="rId1"/>
+    <hyperlink ref="S103" r:id="rId2"/>
+    <hyperlink ref="S104" r:id="rId3"/>
+    <hyperlink ref="S105" r:id="rId4"/>
+    <hyperlink ref="S106" r:id="rId5"/>
+    <hyperlink ref="S107" r:id="rId6"/>
+    <hyperlink ref="S108" r:id="rId7"/>
+    <hyperlink ref="S109" r:id="rId8"/>
+    <hyperlink ref="S110" r:id="rId9"/>
+    <hyperlink ref="S111" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
@@ -10340,7 +10374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10418,7 +10452,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11525,10 +11559,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -12336,7 +12370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C16BBF-19E6-4C8B-9072-1F5646C3351D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">

</xml_diff>

<commit_message>
Scripts added for New member
</commit_message>
<xml_diff>
--- a/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_NewMember\src\main\java\com\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6266E28E-3223-48E9-A898-1238EE6298ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="ApplicationStatusCenter" sheetId="6" r:id="rId2"/>
     <sheet name="Data" sheetId="2" r:id="rId3"/>
-    <sheet name="DNA_Upgrade" sheetId="3" r:id="rId4"/>
-    <sheet name="ProdData" sheetId="4" r:id="rId5"/>
-    <sheet name="DataTwo" sheetId="5" r:id="rId6"/>
-    <sheet name="HomePage" sheetId="7" r:id="rId7"/>
+    <sheet name="Miscellaneous" sheetId="8" r:id="rId4"/>
+    <sheet name="DNA_Upgrade" sheetId="3" r:id="rId5"/>
+    <sheet name="ProdData" sheetId="4" r:id="rId6"/>
+    <sheet name="DataTwo" sheetId="5" r:id="rId7"/>
+    <sheet name="HomePage" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2924" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3070" uniqueCount="597">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1794,12 +1801,36 @@
   </si>
   <si>
     <t>45688744</t>
+  </si>
+  <si>
+    <t>C28355_VerifyDisclouserStepIsHighLightedWhenUserOnIdentityVerification</t>
+  </si>
+  <si>
+    <t>56875658</t>
+  </si>
+  <si>
+    <t>C28357_VerifyDisclouserStepIsHighLightedWhenUserOnAgreementsAndDisclouserPage</t>
+  </si>
+  <si>
+    <t>C28359_VerifyThatDisclousertabIsHighlightedWhenUserDeclineTheAgreement</t>
+  </si>
+  <si>
+    <t>C28361_VerifyThatFundingStepIsHighlightedWhenUserOnAccountFundingPage</t>
+  </si>
+  <si>
+    <t>TC001_ValidateTheAditionalLinkAndShowAllFesturedUnderCDSection</t>
+  </si>
+  <si>
+    <t>TC002_ValidateTheAdditionalLinksPresentOnMemberEligibilityPage</t>
+  </si>
+  <si>
+    <t>56875677</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1939,7 +1970,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1991,7 +2022,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2185,18 +2216,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F153"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F159"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153"/>
+    <sheetView topLeftCell="B140" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158:D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4502,167 +4533,257 @@
         <v>7</v>
       </c>
     </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D154" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D155" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>594</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C158" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>595</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B15" r:id="rId13"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B18" r:id="rId16"/>
-    <hyperlink ref="B19" r:id="rId17"/>
-    <hyperlink ref="B20" r:id="rId18"/>
-    <hyperlink ref="B21" r:id="rId19"/>
-    <hyperlink ref="B22" r:id="rId20"/>
-    <hyperlink ref="B23" r:id="rId21"/>
-    <hyperlink ref="B24" r:id="rId22"/>
-    <hyperlink ref="B25" r:id="rId23"/>
-    <hyperlink ref="B26" r:id="rId24"/>
-    <hyperlink ref="B27" r:id="rId25"/>
-    <hyperlink ref="B28" r:id="rId26"/>
-    <hyperlink ref="B29" r:id="rId27"/>
-    <hyperlink ref="B30" r:id="rId28"/>
-    <hyperlink ref="B31" r:id="rId29"/>
-    <hyperlink ref="B32" r:id="rId30"/>
-    <hyperlink ref="B33" r:id="rId31"/>
-    <hyperlink ref="B34" r:id="rId32"/>
-    <hyperlink ref="B35" r:id="rId33"/>
-    <hyperlink ref="B36" r:id="rId34"/>
-    <hyperlink ref="B37" r:id="rId35"/>
-    <hyperlink ref="B38" r:id="rId36"/>
-    <hyperlink ref="B39" r:id="rId37"/>
-    <hyperlink ref="B40" r:id="rId38"/>
-    <hyperlink ref="B41" r:id="rId39"/>
-    <hyperlink ref="B42" r:id="rId40"/>
-    <hyperlink ref="B43" r:id="rId41"/>
-    <hyperlink ref="B44" r:id="rId42"/>
-    <hyperlink ref="B45" r:id="rId43"/>
-    <hyperlink ref="B46" r:id="rId44"/>
-    <hyperlink ref="B47" r:id="rId45"/>
-    <hyperlink ref="B48" r:id="rId46"/>
-    <hyperlink ref="B49" r:id="rId47"/>
-    <hyperlink ref="B50" r:id="rId48"/>
-    <hyperlink ref="B51" r:id="rId49"/>
-    <hyperlink ref="B52" r:id="rId50"/>
-    <hyperlink ref="B53" r:id="rId51"/>
-    <hyperlink ref="B54" r:id="rId52"/>
-    <hyperlink ref="B55" r:id="rId53"/>
-    <hyperlink ref="B56" r:id="rId54"/>
-    <hyperlink ref="B57" r:id="rId55"/>
-    <hyperlink ref="B58" r:id="rId56"/>
-    <hyperlink ref="B59" r:id="rId57"/>
-    <hyperlink ref="B60" r:id="rId58"/>
-    <hyperlink ref="B61" r:id="rId59"/>
-    <hyperlink ref="B62" r:id="rId60"/>
-    <hyperlink ref="B63" r:id="rId61"/>
-    <hyperlink ref="B64" r:id="rId62"/>
-    <hyperlink ref="B65" r:id="rId63"/>
-    <hyperlink ref="B66" r:id="rId64"/>
-    <hyperlink ref="B67" r:id="rId65"/>
-    <hyperlink ref="B68" r:id="rId66"/>
-    <hyperlink ref="B69" r:id="rId67"/>
-    <hyperlink ref="B70" r:id="rId68"/>
-    <hyperlink ref="B71" r:id="rId69"/>
-    <hyperlink ref="B72" r:id="rId70"/>
-    <hyperlink ref="B73" r:id="rId71"/>
-    <hyperlink ref="B74" r:id="rId72"/>
-    <hyperlink ref="B75" r:id="rId73"/>
-    <hyperlink ref="B76" r:id="rId74"/>
-    <hyperlink ref="B77" r:id="rId75"/>
-    <hyperlink ref="B78" r:id="rId76"/>
-    <hyperlink ref="B79" r:id="rId77"/>
-    <hyperlink ref="B80" r:id="rId78"/>
-    <hyperlink ref="B81" r:id="rId79"/>
-    <hyperlink ref="B82" r:id="rId80"/>
-    <hyperlink ref="B83" r:id="rId81"/>
-    <hyperlink ref="B84" r:id="rId82"/>
-    <hyperlink ref="B85" r:id="rId83"/>
-    <hyperlink ref="B86" r:id="rId84"/>
-    <hyperlink ref="B88" r:id="rId85"/>
-    <hyperlink ref="B89" r:id="rId86"/>
-    <hyperlink ref="B90" r:id="rId87"/>
-    <hyperlink ref="B91" r:id="rId88"/>
-    <hyperlink ref="B92" r:id="rId89"/>
-    <hyperlink ref="B87" r:id="rId90"/>
-    <hyperlink ref="B93" r:id="rId91"/>
-    <hyperlink ref="B94" r:id="rId92"/>
-    <hyperlink ref="B95" r:id="rId93"/>
-    <hyperlink ref="B96" r:id="rId94"/>
-    <hyperlink ref="B97" r:id="rId95"/>
-    <hyperlink ref="B98" r:id="rId96"/>
-    <hyperlink ref="B99" r:id="rId97"/>
-    <hyperlink ref="B100" r:id="rId98"/>
-    <hyperlink ref="B101" r:id="rId99"/>
-    <hyperlink ref="B102" r:id="rId100"/>
-    <hyperlink ref="B103" r:id="rId101"/>
-    <hyperlink ref="B104" r:id="rId102"/>
-    <hyperlink ref="B105" r:id="rId103"/>
-    <hyperlink ref="B106" r:id="rId104"/>
-    <hyperlink ref="B107" r:id="rId105"/>
-    <hyperlink ref="B108" r:id="rId106"/>
-    <hyperlink ref="B109" r:id="rId107"/>
-    <hyperlink ref="B110" r:id="rId108"/>
-    <hyperlink ref="B111" r:id="rId109"/>
-    <hyperlink ref="B112" r:id="rId110"/>
-    <hyperlink ref="B113" r:id="rId111"/>
-    <hyperlink ref="B114" r:id="rId112"/>
-    <hyperlink ref="B115" r:id="rId113"/>
-    <hyperlink ref="B116" r:id="rId114"/>
-    <hyperlink ref="B117" r:id="rId115"/>
-    <hyperlink ref="B118" r:id="rId116"/>
-    <hyperlink ref="B119" r:id="rId117"/>
-    <hyperlink ref="B120" r:id="rId118"/>
-    <hyperlink ref="B121" r:id="rId119"/>
-    <hyperlink ref="B122" r:id="rId120"/>
-    <hyperlink ref="B123" r:id="rId121"/>
-    <hyperlink ref="B124" r:id="rId122"/>
-    <hyperlink ref="B125" r:id="rId123"/>
-    <hyperlink ref="B126" r:id="rId124"/>
-    <hyperlink ref="B127" r:id="rId125"/>
-    <hyperlink ref="B128" r:id="rId126"/>
-    <hyperlink ref="B129" r:id="rId127"/>
-    <hyperlink ref="B130" r:id="rId128"/>
-    <hyperlink ref="B131" r:id="rId129"/>
-    <hyperlink ref="B132" r:id="rId130"/>
-    <hyperlink ref="B133" r:id="rId131"/>
-    <hyperlink ref="B134" r:id="rId132"/>
-    <hyperlink ref="B135" r:id="rId133"/>
-    <hyperlink ref="B136" r:id="rId134"/>
-    <hyperlink ref="B137" r:id="rId135"/>
-    <hyperlink ref="B138" r:id="rId136"/>
-    <hyperlink ref="B139" r:id="rId137"/>
-    <hyperlink ref="B140" r:id="rId138"/>
-    <hyperlink ref="B141" r:id="rId139"/>
-    <hyperlink ref="B142" r:id="rId140"/>
-    <hyperlink ref="B143" r:id="rId141"/>
-    <hyperlink ref="B144" r:id="rId142"/>
-    <hyperlink ref="B145" r:id="rId143"/>
-    <hyperlink ref="B146" r:id="rId144"/>
-    <hyperlink ref="B147" r:id="rId145"/>
-    <hyperlink ref="B148" r:id="rId146"/>
-    <hyperlink ref="B149" r:id="rId147"/>
-    <hyperlink ref="B150" r:id="rId148"/>
-    <hyperlink ref="B151" r:id="rId149"/>
-    <hyperlink ref="B152" r:id="rId150"/>
-    <hyperlink ref="B153" r:id="rId151"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B87" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B94" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B101" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B102" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B103" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B104" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B105" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B106" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B107" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B108" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B109" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B110" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B111" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B112" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B113" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B114" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B115" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B116" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B117" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B118" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B119" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B120" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B121" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B122" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B123" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B124" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B125" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B126" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B127" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B128" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B129" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B130" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B131" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B132" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B133" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B134" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B135" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B136" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B137" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B138" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B139" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="B140" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B141" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="B142" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B143" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="B144" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B145" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="B146" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B147" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="B148" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B149" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="B150" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B151" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="B152" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B153" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="B154" r:id="rId152" xr:uid="{F9B42C70-9C06-4811-B4E5-5F12A2041DFF}"/>
+    <hyperlink ref="B155" r:id="rId153" xr:uid="{FB19BEB6-4E77-4501-A64A-7C8FE7264617}"/>
+    <hyperlink ref="B156" r:id="rId154" xr:uid="{66B4BD23-2638-473E-B97A-2A99F6BF8261}"/>
+    <hyperlink ref="B157" r:id="rId155" xr:uid="{42C89DEB-6E22-4CCD-986E-A09636AC697D}"/>
+    <hyperlink ref="B158" r:id="rId156" xr:uid="{6AF4CA40-A106-4EEF-AEA6-17826A20C19F}"/>
+    <hyperlink ref="B159" r:id="rId157" xr:uid="{66AD87C8-A0D0-4637-8947-ABE537676215}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId152"/>
+  <pageSetup orientation="portrait" r:id="rId158"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4740,8 +4861,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4749,12 +4870,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AE115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE14" sqref="AE14"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93:XFD93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10355,26 +10476,451 @@
         <v>558</v>
       </c>
     </row>
+    <row r="112" spans="1:31" s="6" customFormat="1">
+      <c r="A112" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J112" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K112" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M112" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N112" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="O112" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P112" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q112" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="R112" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S112" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="T112" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE112" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="113" spans="1:31">
+      <c r="A113" t="s">
+        <v>591</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J113" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K113" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L113" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M113" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N113" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="O113" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P113" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q113" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="R113" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S113" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="T113" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U113" s="6"/>
+      <c r="V113" s="6"/>
+      <c r="W113" s="6"/>
+      <c r="X113" s="6"/>
+      <c r="Y113" s="6"/>
+      <c r="Z113" s="6"/>
+      <c r="AA113" s="6"/>
+      <c r="AB113" s="6"/>
+      <c r="AC113" s="6"/>
+      <c r="AD113" s="6"/>
+      <c r="AE113" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="114" spans="1:31">
+      <c r="A114" t="s">
+        <v>592</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J114" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K114" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L114" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N114" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="O114" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P114" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q114" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="R114" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S114" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="T114" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U114" s="6"/>
+      <c r="V114" s="6"/>
+      <c r="W114" s="6"/>
+      <c r="X114" s="6"/>
+      <c r="Y114" s="6"/>
+      <c r="Z114" s="6"/>
+      <c r="AA114" s="6"/>
+      <c r="AB114" s="6"/>
+      <c r="AC114" s="6"/>
+      <c r="AD114" s="6"/>
+      <c r="AE114" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="115" spans="1:31" s="6" customFormat="1">
+      <c r="A115" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="J115" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K115" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L115" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M115" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N115" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O115" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P115" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q115" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R115" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S115" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="T115" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X115" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y115" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z115" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE115" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S102" r:id="rId1"/>
-    <hyperlink ref="S103" r:id="rId2"/>
-    <hyperlink ref="S104" r:id="rId3"/>
-    <hyperlink ref="S105" r:id="rId4"/>
-    <hyperlink ref="S106" r:id="rId5"/>
-    <hyperlink ref="S107" r:id="rId6"/>
-    <hyperlink ref="S108" r:id="rId7"/>
-    <hyperlink ref="S109" r:id="rId8"/>
-    <hyperlink ref="S110" r:id="rId9"/>
-    <hyperlink ref="S111" r:id="rId10"/>
+    <hyperlink ref="S102" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="S103" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="S104" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="S105" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="S106" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="S107" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="S108" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="S109" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="S110" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="S111" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="S112" r:id="rId11" xr:uid="{DF7B14E4-8213-4A5F-AF26-BA81B4495527}"/>
+    <hyperlink ref="S113" r:id="rId12" xr:uid="{85B6BC87-1724-4C07-A2C8-086BC4C676E1}"/>
+    <hyperlink ref="S114" r:id="rId13" xr:uid="{348F2698-E65A-4B4C-9C4A-8D971F97E312}"/>
+    <hyperlink ref="S115" r:id="rId14" xr:uid="{2C7775BE-2D15-4E90-87DD-AF2B85FF4A01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA266BC-709C-4DEE-8391-B55B5482C45E}">
+  <dimension ref="A1:AE3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
+      <c r="A2" s="6" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="6" customFormat="1">
+      <c r="A3" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10451,8 +10997,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11558,8 +12104,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -12369,8 +12915,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">

</xml_diff>

<commit_message>
C26854 and C26856 Test Cases
C26854 Complete
C26856 In Progress
</commit_message>
<xml_diff>
--- a/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_NewMember\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CorpData\TDECU\TDECUProjects\InstantOpen_NewMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6266E28E-3223-48E9-A898-1238EE6298ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57B8245-3011-4961-A223-5B1C207C26EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3070" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3078" uniqueCount="599">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1825,6 +1825,12 @@
   </si>
   <si>
     <t>56875677</t>
+  </si>
+  <si>
+    <t>C26854_VerifyCheckingSavingsAndCDsSection</t>
+  </si>
+  <si>
+    <t>C26856_Verify_HelpModal_HomePage</t>
   </si>
 </sst>
 </file>
@@ -2224,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F159"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView topLeftCell="B140" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158:D159"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4614,6 +4620,34 @@
         <v>5</v>
       </c>
       <c r="D159" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" t="s">
+        <v>597</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D160" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" t="s">
+        <v>598</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D162" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4776,9 +4810,11 @@
     <hyperlink ref="B157" r:id="rId155" xr:uid="{42C89DEB-6E22-4CCD-986E-A09636AC697D}"/>
     <hyperlink ref="B158" r:id="rId156" xr:uid="{6AF4CA40-A106-4EEF-AEA6-17826A20C19F}"/>
     <hyperlink ref="B159" r:id="rId157" xr:uid="{66AD87C8-A0D0-4637-8947-ABE537676215}"/>
+    <hyperlink ref="B160" r:id="rId158" xr:uid="{A5786DE6-087D-4CEC-8CB8-7DD728DC50C0}"/>
+    <hyperlink ref="B162" r:id="rId159" xr:uid="{B88C4656-4950-4237-858B-8C3B64A7B110}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId158"/>
+  <pageSetup orientation="portrait" r:id="rId160"/>
 </worksheet>
 </file>
 
@@ -10743,7 +10779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA266BC-709C-4DEE-8391-B55B5482C45E}">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -12917,10 +12953,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12959,6 +12995,9 @@
         <v>587</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Code Commit for Test Case ID C24321
</commit_message>
<xml_diff>
--- a/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CorpData\Lavanya\TDECU Projects\TDECUProjects\InstantOpen_NewMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E714F7-181C-4AB9-BA84-61CAEF0878F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5052DDAE-EF68-4B91-BFC9-50CB89A7969B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3205" uniqueCount="615">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1871,6 +1871,15 @@
   </si>
   <si>
     <t>51411589</t>
+  </si>
+  <si>
+    <t>C24321_NonMemberUserCanSeeTheAssignedRoleToTheBeneficiary</t>
+  </si>
+  <si>
+    <t>ConfirmAccountRoles</t>
+  </si>
+  <si>
+    <t>This application has multiple individuals. By default all individuals have roles on accounts on the application. To remove an individual from one or more accounts you can un-check the account for that individual.</t>
   </si>
 </sst>
 </file>
@@ -2282,10 +2291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4756,6 +4765,20 @@
         <v>5</v>
       </c>
       <c r="D167" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="s">
+        <v>612</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D168" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4924,9 +4947,10 @@
     <hyperlink ref="B165" r:id="rId161" xr:uid="{B396CB91-CA01-4EDC-9E64-6F68FC829D3F}"/>
     <hyperlink ref="B166" r:id="rId162" xr:uid="{6112E321-2B5C-458B-8B69-EA037E40FF14}"/>
     <hyperlink ref="B167" r:id="rId163" xr:uid="{16604E5A-DCA8-4226-8AFA-B79AD4A08261}"/>
+    <hyperlink ref="B168" r:id="rId164" xr:uid="{F7CCC421-26CE-40DD-8A46-67E3A214002A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId164"/>
+  <pageSetup orientation="portrait" r:id="rId165"/>
 </worksheet>
 </file>
 
@@ -5019,11 +5043,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AE116"/>
+  <dimension ref="A1:AF117"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5052,9 +5076,10 @@
     <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="195.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="3" customFormat="1">
+    <row r="1" spans="1:32" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5148,8 +5173,11 @@
       <c r="AE1" s="3" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="2" spans="1:31">
+      <c r="AF1" s="3" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -5206,7 +5234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -5223,7 +5251,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="6" customFormat="1">
+    <row r="4" spans="1:32" s="6" customFormat="1">
       <c r="A4" s="6" t="s">
         <v>48</v>
       </c>
@@ -5240,7 +5268,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="6" customFormat="1">
+    <row r="5" spans="1:32" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -5263,7 +5291,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:32">
       <c r="A6" s="6" t="s">
         <v>54</v>
       </c>
@@ -5280,7 +5308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="44.25" customHeight="1">
+    <row r="7" spans="1:32" ht="44.25" customHeight="1">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -5300,7 +5328,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:32">
       <c r="A8" s="6" t="s">
         <v>86</v>
       </c>
@@ -5320,7 +5348,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:32">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -5328,7 +5356,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:32">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -5348,7 +5376,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:32">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -5368,7 +5396,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:32">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -5387,7 +5415,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:32">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -5402,7 +5430,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:32">
       <c r="A14" s="6" t="s">
         <v>92</v>
       </c>
@@ -5473,7 +5501,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:32">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -5541,7 +5569,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:32">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -10677,7 +10705,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="113" spans="1:31">
+    <row r="113" spans="1:32">
       <c r="A113" t="s">
         <v>591</v>
       </c>
@@ -10740,7 +10768,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="114" spans="1:31">
+    <row r="114" spans="1:32">
       <c r="A114" t="s">
         <v>592</v>
       </c>
@@ -10803,7 +10831,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="115" spans="1:31" s="6" customFormat="1">
+    <row r="115" spans="1:32" s="6" customFormat="1">
       <c r="A115" s="6" t="s">
         <v>593</v>
       </c>
@@ -10865,9 +10893,85 @@
         <v>558</v>
       </c>
     </row>
-    <row r="116" spans="1:31">
+    <row r="116" spans="1:32">
       <c r="A116" t="s">
         <v>601</v>
+      </c>
+    </row>
+    <row r="117" spans="1:32">
+      <c r="A117" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J117" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K117" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L117" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M117" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N117" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O117" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P117" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q117" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R117" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S117" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T117" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U117" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="V117" s="2"/>
+      <c r="W117" s="6"/>
+      <c r="X117" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y117" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z117" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA117" s="6"/>
+      <c r="AB117" s="6"/>
+      <c r="AC117" s="6"/>
+      <c r="AD117" s="6"/>
+      <c r="AE117" s="6"/>
+      <c r="AF117" s="2" t="s">
+        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -11095,6 +11199,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11173,6 +11278,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12287,7 +12393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -13170,7 +13276,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13464,6 +13570,6 @@
     <hyperlink ref="V2" r:id="rId1" display="mailto:TestW@emailaddress.com" xr:uid="{EA6F4A22-163B-4E81-877C-C02FF484E208}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code Complete for C24321
</commit_message>
<xml_diff>
--- a/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_NewMember/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aditip\Documents\reference\tdecu\projects\TDECUProjects\InstantOpen_NewMember\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CorpData\Lavanya\TDECU Projects\TDECUProjects\InstantOpen_NewMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545D2124-5BBF-4918-9C2D-FCA0C9AE41CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD99CE1-A0F3-48EF-AE1E-4784EB4E6D53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,25 @@
     <sheet name="HomePage_Data" sheetId="10" r:id="rId9"/>
     <sheet name="StaticUIdata" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3278" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3278" uniqueCount="654">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -2002,6 +2010,9 @@
   </si>
   <si>
     <t>C26855_VerifyLoanCreditCardCriteriaDetails</t>
+  </si>
+  <si>
+    <t>1132888</t>
   </si>
 </sst>
 </file>
@@ -2095,11 +2106,11 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2418,7 +2429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+    <sheetView topLeftCell="A145" workbookViewId="0">
       <selection activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
@@ -5332,9 +5343,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AF117"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F124" sqref="F124"/>
+      <selection pane="bottomLeft" activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11200,7 +11211,7 @@
         <v>29</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>496</v>
+        <v>653</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>46</v>
@@ -13660,13 +13671,13 @@
       <c r="G4" s="12" t="s">
         <v>641</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>642</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>642</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>643</v>
       </c>
       <c r="K4" s="12" t="s">
@@ -13737,11 +13748,11 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>602</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>